<commit_message>
Changed energy in Joule
</commit_message>
<xml_diff>
--- a/final_eigenvec_two.xlsx
+++ b/final_eigenvec_two.xlsx
@@ -457,58 +457,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3.973817185632454e-09</v>
+        <v>-2.270752701386355e-09</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.4999999995156539</v>
+        <v>7.947634585102704e-09</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7071067875841902</v>
+        <v>-2.947695123254957e-16</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5000000128792476</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B3" t="n">
-        <v>3.973817268174947e-09</v>
+        <v>-1.145081752690021e-17</v>
       </c>
       <c r="C3" t="n">
-        <v>7.223969875409575e-17</v>
+        <v>-2.649211528367555e-09</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.973817373400877e-09</v>
+        <v>-2.270752701386034e-09</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-1.711121786372764e-16</v>
+        <v>3.205366103897332e-16</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.707106788215934</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>3.175162366649175e-09</v>
+        <v>-1.589526917020532e-08</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.7071067694918804</v>
+        <v>-7.947634585102661e-09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.973817292551333e-09</v>
+        <v>-2.649211528367557e-09</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4999999905432921</v>
+        <v>1.589526917020536e-08</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7071067747889048</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5000000036595091</v>
+        <v>1.624240170942698e-16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to Advantage QPU
</commit_message>
<xml_diff>
--- a/final_eigenvec_two.xlsx
+++ b/final_eigenvec_two.xlsx
@@ -457,58 +457,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-2.270752701386355e-09</v>
+        <v>1.139856140145738e-19</v>
       </c>
       <c r="B2" t="n">
-        <v>7.947634585102704e-09</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.947695123254957e-16</v>
+        <v>4.828585634557355e-10</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>-3.219057405581146e-10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>1.931434253822948e-10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4.828585634557358e-10</v>
+      </c>
+      <c r="C3" t="n">
         <v>-1</v>
       </c>
-      <c r="B3" t="n">
-        <v>-1.145081752690021e-17</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-2.649211528367555e-09</v>
-      </c>
       <c r="D3" t="n">
-        <v>-2.270752701386034e-09</v>
+        <v>-1.22328035736726e-16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.205366103897332e-16</v>
+        <v>1.609528544852451e-10</v>
       </c>
       <c r="B4" t="n">
+        <v>3.219058626773073e-10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-6.717089639404731e-16</v>
+      </c>
+      <c r="D4" t="n">
         <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-1.589526917020532e-08</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-7.947634585102661e-09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-2.649211528367557e-09</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>1.589526917020536e-08</v>
+        <v>-2.590582384090349e-19</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>1.931434253822923e-10</v>
       </c>
       <c r="D5" t="n">
-        <v>1.624240170942698e-16</v>
+        <v>-1.609528544852464e-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>